<commit_message>
#332 Update documentation (due to modularization)
- Fix missing code tags (from 312)
- Fix xrefs for the misc. target docs (site/html5/PDF)
- Update/refactor outdated external URLs
- Fix missing attributes
- Drop JCenter in favor of Maven Central (and JitPack (321)
- Partially align formatting of adoc according to good practices
- Use SVGs in favor of PNGs for PlantUML
- Fix some typos, grammar etc.
- Treat 429 response codes during external link checking as success (it only means there is some rate limiting in place)
- Make the page location in HTML reports a hyperlink
</commit_message>
<xml_diff>
--- a/src/docs/Requirements.xlsx
+++ b/src/docs/Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ralfd\projects\github\docToolchainMaster\htmlSanityCheck\src\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerd.aschemann/wrk/aim42/htmlSanityCheck/src/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE84764-FDB6-4EC4-9039-A442FE0E2ED3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A58F7B-CD5B-D54B-A171-F9C8EACAE148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23451" windowHeight="11494" xr2:uid="{F85F13AA-3926-4838-A581-AF1A5241F0CA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23460" windowHeight="11500" xr2:uid="{F85F13AA-3926-4838-A581-AF1A5241F0CA}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -203,9 +203,6 @@
     <t>available via public repositories</t>
   </si>
   <si>
-    <t>like bintray or jcenter.</t>
-  </si>
-  <si>
     <t>G-7</t>
   </si>
   <si>
@@ -348,6 +345,9 @@
   </si>
   <si>
     <t>{gradle-url}-plugin</t>
+  </si>
+  <si>
+    <t>Maven Central</t>
   </si>
 </sst>
 </file>
@@ -408,30 +408,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -447,7 +444,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -746,101 +743,101 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="35.07421875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.69140625" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="6" t="s">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="5" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -856,110 +853,110 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.3828125" customWidth="1"/>
-    <col min="3" max="3" width="77.765625" customWidth="1"/>
+    <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="77.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C3" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="7" t="s">
+    <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C4" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="7" t="s">
+    <row r="5" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="B5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="7" t="s">
+    <row r="6" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="B6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    <row r="8" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -975,43 +972,43 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1027,54 +1024,54 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.84375" customWidth="1"/>
-    <col min="2" max="2" width="20.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.3046875" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1091,99 +1088,98 @@
       <selection activeCell="C8" sqref="A2:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.3046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.61328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="114.69140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.07421875" style="1"/>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="114.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="8">
+    <row r="2" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="8">
+    <row r="3" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="8">
+    <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="8">
+    <row r="5" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="8">
+    <row r="6" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
         <v>2</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="8">
+    <row r="7" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
         <v>2</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="8">
+    <row r="8" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
         <v>3</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#332 Fix cross references
</commit_message>
<xml_diff>
--- a/src/docs/Requirements.xlsx
+++ b/src/docs/Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerd.aschemann/wrk/aim42/htmlSanityCheck/src/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ascheman/wrk/aim42/htmlSanityCheck/src/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A58F7B-CD5B-D54B-A171-F9C8EACAE148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798CC31E-1F6F-EB4E-895C-CDB61B49AB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23460" windowHeight="11500" xr2:uid="{F85F13AA-3926-4838-A581-AF1A5241F0CA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{F85F13AA-3926-4838-A581-AF1A5241F0CA}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -209,12 +209,6 @@
     <t>configurable to check multiple HTML files</t>
   </si>
   <si>
-    <t>HtmlSC shall read a single (configurable) HTML file</t>
-  </si>
-  <si>
-    <t>HtmlSC can be called from the command line with arguments and options</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">configure a set of files to be processes in a single </t>
     </r>
@@ -305,21 +299,6 @@
     </r>
   </si>
   <si>
-    <t>Check all image tags if the referenced image files exist. See &lt;&lt;MissingImageFilesChecker&gt;&gt;</t>
-  </si>
-  <si>
-    <t>Check all internal links from anchor-tags (href="#XYZ") if the link targets "XYZ" are defined. See &lt;&lt;BrokenCrossReferencesChecker&gt;&gt;</t>
-  </si>
-  <si>
-    <t>either other html-files, pdf’s or similar. See &lt;&lt;MissingLocalResourcesChecker&gt;&gt;</t>
-  </si>
-  <si>
-    <t>Check all bookmark definitions (…​ id="XYZ") whether the id’s ("XYZ") are unique. See &lt;&lt;DuplicateIdChecker&gt;&gt;</t>
-  </si>
-  <si>
-    <t>in image-tags. See &lt;&lt;MissingImgAltAttributeChecker&gt;&gt;</t>
-  </si>
-  <si>
     <t>Opt-1</t>
   </si>
   <si>
@@ -341,13 +320,34 @@
     <t>all required dependencies shall be compliant to the https://creativecommons.org/licenses/by-sa/4.0/[CC-SA-4 licence].</t>
   </si>
   <si>
-    <t>HtmlSC can be run as {gradle-url}-plugin.</t>
-  </si>
-  <si>
     <t>{gradle-url}-plugin</t>
   </si>
   <si>
     <t>Maven Central</t>
+  </si>
+  <si>
+    <t>Check all internal links from anchor-tags (href="#XYZ") if the link targets "XYZ" are defined. See {xrefAlgorithmBrokenCrossReferencesChecker}</t>
+  </si>
+  <si>
+    <t>Check all image tags if the referenced image files exist. See {xrefAlgorithmMissingImageFilesChecker}</t>
+  </si>
+  <si>
+    <t>either other html-files, pdf’s or similar. See {xrefAlgorithmMissingLocalResourcesChecker}</t>
+  </si>
+  <si>
+    <t>Check all bookmark definitions (…​ id="XYZ") whether the id’s ("XYZ") are unique. See {xrefAlgorithmDuplicateIdChecker}</t>
+  </si>
+  <si>
+    <t>in image-tags. See {xrefAlgorithmMissingImgAltAttributeChecker}</t>
+  </si>
+  <si>
+    <t>HSC shall read a single (configurable) HTML file</t>
+  </si>
+  <si>
+    <t>HSC can be run as {gradle-url}-plugin.</t>
+  </si>
+  <si>
+    <t>HSC can be called from the command line with arguments and options</t>
   </si>
 </sst>
 </file>
@@ -444,9 +444,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -484,7 +484,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -590,7 +590,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -732,7 +732,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790DAFB9-3809-45AB-9D4E-BB72FEF9941B}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -771,7 +771,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -779,10 +779,10 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
         <v>74</v>
-      </c>
-      <c r="C3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -793,7 +793,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -815,7 +815,7 @@
         <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -826,7 +826,7 @@
         <v>38</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -837,7 +837,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -849,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D28D2816-508C-45E4-8169-53E3E9D9FF78}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -865,7 +865,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>16</v>
@@ -876,10 +876,10 @@
         <v>17</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -887,10 +887,10 @@
         <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -898,65 +898,65 @@
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -983,7 +983,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>16</v>
@@ -991,24 +991,24 @@
     </row>
     <row r="2" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1085,7 +1085,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="A2:C8"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>